<commit_message>
added averaging during impulses for each channel
was only able to do it for the hilbert transform at MRM1. Need to do for the rectified, and do duplicate analysis for MRM2.
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/manual_calibrations_combined_V2.xlsx
+++ b/Hydrophones/Calibration/manual_calibrations_combined_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41303F0-70DA-4201-90E7-4FA555115F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8B869D-2B6C-409C-814D-B57331719945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hilbert envelope" sheetId="1" r:id="rId1"/>
@@ -23971,8 +23971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25544,8 +25544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CBDE796-D6C4-41DF-BB85-D95E6EE6B828}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AG13" sqref="AG13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>